<commit_message>
Se agrego hora de levantada de julio y de victico
</commit_message>
<xml_diff>
--- a/Seguimiento.xlsx
+++ b/Seguimiento.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>17/04:22</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>durante la noche encendi el ventilador para dormir, sin tocar el televisor ni aire.</t>
+  </si>
+  <si>
+    <t>me desperté a las 7:00 am, el ventilador estuvo encendido hasta las 07:30</t>
   </si>
 </sst>
 </file>
@@ -66,13 +69,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,11 +103,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F43"/>
+  <dimension ref="A3:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
@@ -698,7 +707,13 @@
         <v>10</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>